<commit_message>
mise à jour contraintesBD
</commit_message>
<xml_diff>
--- a/ContraintesBD.xlsx
+++ b/ContraintesBD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>ContraintesBD</t>
   </si>
@@ -89,16 +89,26 @@
     <t>je m'en charge !</t>
   </si>
   <si>
-    <t>Before Insert On Ligne</t>
-  </si>
-  <si>
-    <t>Before Insert On Bille</t>
-  </si>
-  <si>
     <t>Before Insert On Combinaison</t>
   </si>
   <si>
     <t>Pierrick</t>
+  </si>
+  <si>
+    <t>Before Insert On PropositionJoueur</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>tester nombre emplacements billes
+et nombre effectif de bille</t>
+  </si>
+  <si>
+    <t>After Insert On Partie</t>
+  </si>
+  <si>
+    <t>créer une combinaison avec aucune bille en double</t>
   </si>
 </sst>
 </file>
@@ -176,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -199,6 +209,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +506,7 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="76" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,10 +548,10 @@
         <v>17</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,21 +581,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -587,7 +603,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -598,7 +614,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -636,7 +652,15 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
màj to do list pierrick
</commit_message>
<xml_diff>
--- a/ContraintesBD.xlsx
+++ b/ContraintesBD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>ContraintesBD</t>
   </si>
@@ -498,7 +498,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,6 +591,9 @@
       <c r="D9" s="10" t="s">
         <v>25</v>
       </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
ancien site web et suppresion ancienne photo bd
</commit_message>
<xml_diff>
--- a/ContraintesBD.xlsx
+++ b/ContraintesBD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>ContraintesBD</t>
   </si>
@@ -118,6 +118,186 @@
   </si>
   <si>
     <t>Natchley</t>
+  </si>
+  <si>
+    <t>Bille</t>
+  </si>
+  <si>
+    <t>Historique</t>
+  </si>
+  <si>
+    <t>CategorieJoueur</t>
+  </si>
+  <si>
+    <t>Niveau</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>Joueur</t>
+  </si>
+  <si>
+    <t>Partie</t>
+  </si>
+  <si>
+    <t>Ligne</t>
+  </si>
+  <si>
+    <t>Combinaison</t>
+  </si>
+  <si>
+    <t>Debloquer</t>
+  </si>
+  <si>
+    <t>Proposition_Joueur</t>
+  </si>
+  <si>
+    <t>Jouer</t>
+  </si>
+  <si>
+    <t>Composer</t>
+  </si>
+  <si>
+    <t>idBilles</t>
+  </si>
+  <si>
+    <t>idHistorique</t>
+  </si>
+  <si>
+    <t>nomCat</t>
+  </si>
+  <si>
+    <t>imageCat</t>
+  </si>
+  <si>
+    <t>idCat</t>
+  </si>
+  <si>
+    <t>urlB</t>
+  </si>
+  <si>
+    <t>idNiveau</t>
+  </si>
+  <si>
+    <t>seuilExpN</t>
+  </si>
+  <si>
+    <t>nbEmplacementsN</t>
+  </si>
+  <si>
+    <t>timerN</t>
+  </si>
+  <si>
+    <t>idCollectionN</t>
+  </si>
+  <si>
+    <t>idJoueur</t>
+  </si>
+  <si>
+    <t>pseudoJ</t>
+  </si>
+  <si>
+    <t>experienceJ</t>
+  </si>
+  <si>
+    <t>motDePasseJ</t>
+  </si>
+  <si>
+    <t>idCollection</t>
+  </si>
+  <si>
+    <t>nomCol</t>
+  </si>
+  <si>
+    <t>nbBillesCol</t>
+  </si>
+  <si>
+    <t>difficulteBillesCol</t>
+  </si>
+  <si>
+    <t>idPartie</t>
+  </si>
+  <si>
+    <t>scoreP</t>
+  </si>
+  <si>
+    <t>dateP</t>
+  </si>
+  <si>
+    <t>resultatP</t>
+  </si>
+  <si>
+    <t>idLigneL</t>
+  </si>
+  <si>
+    <t>numeroL</t>
+  </si>
+  <si>
+    <t>tempsLigneL</t>
+  </si>
+  <si>
+    <t>idBille</t>
+  </si>
+  <si>
+    <t>positionBilleCombinaison</t>
+  </si>
+  <si>
+    <t>positionBilleLigne</t>
+  </si>
+  <si>
+    <t>motDePasse</t>
+  </si>
+  <si>
+    <t>images/billesDures</t>
+  </si>
+  <si>
+    <t>images/billesFaciles</t>
+  </si>
+  <si>
+    <t>images/billesClassique</t>
+  </si>
+  <si>
+    <t>HommesPolitiques</t>
+  </si>
+  <si>
+    <t>CouleursClassiques</t>
+  </si>
+  <si>
+    <t>CouleursFlashies</t>
+  </si>
+  <si>
+    <t>bronze</t>
+  </si>
+  <si>
+    <t>argent</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>imageCat/bronze</t>
+  </si>
+  <si>
+    <t>imageCat/argent</t>
+  </si>
+  <si>
+    <t>imageCat/or</t>
+  </si>
+  <si>
+    <t>facile</t>
+  </si>
+  <si>
+    <t>difficile</t>
+  </si>
+  <si>
+    <t>moyenne</t>
+  </si>
+  <si>
+    <t>azertty123</t>
+  </si>
+  <si>
+    <t>yoloGuy</t>
   </si>
 </sst>
 </file>
@@ -202,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -232,6 +412,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +705,11 @@
     <col min="2" max="2" width="76" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,6 +901,499 @@
         <v>30</v>
       </c>
     </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" t="s">
+        <v>53</v>
+      </c>
+      <c r="I38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>23</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>45</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41" s="13">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" t="s">
+        <v>61</v>
+      </c>
+      <c r="H44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" t="s">
+        <v>56</v>
+      </c>
+      <c r="G50" t="s">
+        <v>57</v>
+      </c>
+      <c r="H50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51">
+        <v>23</v>
+      </c>
+      <c r="H51" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>63</v>
+      </c>
+      <c r="F56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G56" t="s">
+        <v>65</v>
+      </c>
+      <c r="H56" t="s">
+        <v>66</v>
+      </c>
+      <c r="I56" t="s">
+        <v>45</v>
+      </c>
+      <c r="J56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>67</v>
+      </c>
+      <c r="F62" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" t="s">
+        <v>69</v>
+      </c>
+      <c r="H62" t="s">
+        <v>63</v>
+      </c>
+      <c r="I62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G68" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>55</v>
+      </c>
+      <c r="F74" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>72</v>
+      </c>
+      <c r="F80" t="s">
+        <v>67</v>
+      </c>
+      <c r="G80" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>55</v>
+      </c>
+      <c r="F86" t="s">
+        <v>56</v>
+      </c>
+      <c r="G86" t="s">
+        <v>57</v>
+      </c>
+      <c r="H86" t="s">
+        <v>73</v>
+      </c>
+      <c r="I86" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>70</v>
+      </c>
+      <c r="F92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
màj todo list triggers
</commit_message>
<xml_diff>
--- a/ContraintesBD.xlsx
+++ b/ContraintesBD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
   <si>
     <t>ContraintesBD</t>
   </si>
@@ -349,6 +349,13 @@
   </si>
   <si>
     <t>màj de la liste dans le google drive</t>
+  </si>
+  <si>
+    <t>After insert on Joueur</t>
+  </si>
+  <si>
+    <t>on crée  l'historique du joueur après avoir crée le joueur
+idHistorique : joueur + partie + date</t>
   </si>
 </sst>
 </file>
@@ -446,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -479,6 +486,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,7 +840,7 @@
   <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,6 +1139,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
choix de deux triggers à faire
</commit_message>
<xml_diff>
--- a/ContraintesBD.xlsx
+++ b/ContraintesBD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrick Herve\Documents\BDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRO_SITE_BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
   <si>
     <t>ContraintesBD</t>
   </si>
@@ -1111,6 +1111,9 @@
       <c r="D22" t="s">
         <v>107</v>
       </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -1121,6 +1124,9 @@
       </c>
       <c r="D23" t="s">
         <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
billes et état d'avancement contraintes
</commit_message>
<xml_diff>
--- a/ContraintesBD.xlsx
+++ b/ContraintesBD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRO_SITE_BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierrick Herve\Documents\BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="113">
   <si>
     <t>ContraintesBD</t>
   </si>
@@ -356,6 +356,15 @@
   <si>
     <t>on crée  l'historique du joueur après avoir crée le joueur
 idHistorique : joueur + partie + date</t>
+  </si>
+  <si>
+    <t>colonne</t>
+  </si>
+  <si>
+    <t>fait</t>
+  </si>
+  <si>
+    <t>à faire</t>
   </si>
 </sst>
 </file>
@@ -399,7 +408,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,8 +421,14 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -449,11 +464,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,6 +513,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,12 +885,12 @@
     <col min="10" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -875,8 +903,11 @@
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -890,7 +921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -903,8 +934,11 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -915,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -926,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -940,7 +974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -953,8 +987,11 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -971,7 +1008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -984,8 +1021,11 @@
       <c r="E11" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -999,7 +1039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1010,7 +1050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -1035,7 +1075,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>30</v>
       </c>
@@ -1046,7 +1086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -1057,7 +1097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1081,8 +1121,11 @@
       <c r="E19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>37</v>
       </c>
@@ -1093,7 +1136,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>39</v>
       </c>
@@ -1101,7 +1144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -1115,7 +1158,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -1129,7 +1172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>106</v>
       </c>
@@ -1137,7 +1180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>44</v>
       </c>
@@ -1147,8 +1190,11 @@
       <c r="E25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
         <v>109</v>
       </c>
@@ -1161,8 +1207,11 @@
       <c r="E26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>45</v>
       </c>
@@ -1657,6 +1706,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>